<commit_message>
BurnDownChart du Sprint n2
</commit_message>
<xml_diff>
--- a/Scrum/BurndownChart-26.04To10.05.xlsx
+++ b/Scrum/BurndownChart-26.04To10.05.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\P_Catalogue\ma-gu-wa\ma-gu-wa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\P_Catalogue\ma-gu-wa-v2\ma-gu-wa-Git-Flow\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -501,55 +501,55 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1215,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="19">
         <v>0</v>
@@ -1238,15 +1238,33 @@
       <c r="O3" s="19">
         <v>0</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
+      <c r="P3" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>0</v>
+      </c>
+      <c r="R3" s="19">
+        <v>0</v>
+      </c>
+      <c r="S3" s="19">
+        <v>0</v>
+      </c>
+      <c r="T3" s="19">
+        <v>0</v>
+      </c>
+      <c r="U3" s="19">
+        <v>0</v>
+      </c>
+      <c r="V3" s="19">
+        <v>0</v>
+      </c>
+      <c r="W3" s="19">
+        <v>0</v>
+      </c>
+      <c r="X3" s="19">
+        <v>0</v>
+      </c>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
@@ -1276,32 +1294,50 @@
         <v>16</v>
       </c>
       <c r="J4" s="19">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K4" s="19">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L4" s="19">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="M4" s="19">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N4" s="19">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O4" s="19">
-        <v>11</v>
-      </c>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
+        <v>16</v>
+      </c>
+      <c r="P4" s="19">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>16</v>
+      </c>
+      <c r="R4" s="19">
+        <v>16</v>
+      </c>
+      <c r="S4" s="19">
+        <v>16</v>
+      </c>
+      <c r="T4" s="19">
+        <v>16</v>
+      </c>
+      <c r="U4" s="19">
+        <v>16</v>
+      </c>
+      <c r="V4" s="19">
+        <v>16</v>
+      </c>
+      <c r="W4" s="19">
+        <v>16</v>
+      </c>
+      <c r="X4" s="19">
+        <v>0</v>
+      </c>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
@@ -1348,15 +1384,33 @@
       <c r="O5" s="19">
         <v>10</v>
       </c>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
+      <c r="P5" s="19">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>10</v>
+      </c>
+      <c r="R5" s="19">
+        <v>10</v>
+      </c>
+      <c r="S5" s="19">
+        <v>10</v>
+      </c>
+      <c r="T5" s="19">
+        <v>10</v>
+      </c>
+      <c r="U5" s="19">
+        <v>10</v>
+      </c>
+      <c r="V5" s="19">
+        <v>10</v>
+      </c>
+      <c r="W5" s="19">
+        <v>10</v>
+      </c>
+      <c r="X5" s="19">
+        <v>10</v>
+      </c>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
@@ -1386,32 +1440,50 @@
         <v>10</v>
       </c>
       <c r="J6" s="19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K6" s="19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L6" s="19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="M6" s="19">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="N6" s="19">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O6" s="19">
         <v>0</v>
       </c>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
+      <c r="P6" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="19">
+        <v>0</v>
+      </c>
+      <c r="R6" s="19">
+        <v>0</v>
+      </c>
+      <c r="S6" s="19">
+        <v>0</v>
+      </c>
+      <c r="T6" s="19">
+        <v>0</v>
+      </c>
+      <c r="U6" s="19">
+        <v>0</v>
+      </c>
+      <c r="V6" s="19">
+        <v>0</v>
+      </c>
+      <c r="W6" s="19">
+        <v>0</v>
+      </c>
+      <c r="X6" s="19">
+        <v>0</v>
+      </c>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
@@ -1695,7 +1767,7 @@
       </c>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" si="0"/>
@@ -1703,63 +1775,63 @@
       </c>
       <c r="J16" s="6">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K16" s="6">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N16" s="6">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O16" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="P16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="Q16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="S16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="T16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="U16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="V16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="W16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="X16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
@@ -1878,50 +1950,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?><ct:contentTypeSchema ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F770ABC8F9B27C4C8461F4575C23FAEA" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6f0f4afd6cc55b40f57cb0d59e49aa45" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes">
@@ -2098,7 +2127,50 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?><p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"><documentManagement><_dlc_DocId xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07">WORK-769-153</_dlc_DocId><_dlc_DocIdUrl xmlns="0d93dc7d-5998-434b-bf34-aa89b432ec07"><Url>http://intranet/workingtogether/projects/110405/_layouts/DocIdRedir.aspx?ID=WORK-769-153</Url><Description>WORK-769-153</Description></_dlc_DocIdUrl><IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/><Last_x0020_Archive xmlns="$ListId:Shared Documents;" xsi:nil="true"/><Reason xmlns="$ListId:Shared Documents;" xsi:nil="true"></Reason></documentManagement></p:properties>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2110,9 +2182,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F807D2B-FCE5-4B63-BC9A-551BEF173D66}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BCCC64-3980-40D2-8C4F-F5BACE67ECB4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2138,19 +2220,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47BCCC64-3980-40D2-8C4F-F5BACE67ECB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F807D2B-FCE5-4B63-BC9A-551BEF173D66}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="$ListId:Shared Documents;"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0d93dc7d-5998-434b-bf34-aa89b432ec07"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>